<commit_message>
remove others in building
</commit_message>
<xml_diff>
--- a/trans_share_pass.xlsx
+++ b/trans_share_pass.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F193"/>
+  <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,7 +396,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -409,10 +409,10 @@
         </is>
       </c>
       <c r="E2">
-        <v>14116.1</v>
+        <v>85533.39999999999</v>
       </c>
       <c r="F2">
-        <v>23.72764633618808</v>
+        <v>24.31690424481558</v>
       </c>
     </row>
     <row r="3">
@@ -422,7 +422,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -435,10 +435,10 @@
         </is>
       </c>
       <c r="E3">
-        <v>2682.94</v>
+        <v>26724.24</v>
       </c>
       <c r="F3">
-        <v>4.509733670150569</v>
+        <v>7.597626016216711</v>
       </c>
     </row>
     <row r="4">
@@ -448,7 +448,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -461,10 +461,10 @@
         </is>
       </c>
       <c r="E4">
-        <v>4082.4</v>
+        <v>37199</v>
       </c>
       <c r="F4">
-        <v>6.862075460138013</v>
+        <v>10.57557072445261</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -487,10 +487,10 @@
         </is>
       </c>
       <c r="E5">
-        <v>998.735</v>
+        <v>50716.57</v>
       </c>
       <c r="F5">
-        <v>1.67876615096045</v>
+        <v>14.41857772888119</v>
       </c>
     </row>
     <row r="6">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -513,10 +513,10 @@
         </is>
       </c>
       <c r="E6">
-        <v>30093.7</v>
+        <v>92887</v>
       </c>
       <c r="F6">
-        <v>50.58427402379858</v>
+        <v>26.40751197296243</v>
       </c>
     </row>
     <row r="7">
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>1975</v>
+        <v>2015</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -539,10 +539,10 @@
         </is>
       </c>
       <c r="E7">
-        <v>7518.33</v>
+        <v>58684.4</v>
       </c>
       <c r="F7">
-        <v>12.63750435876431</v>
+        <v>16.68380931267149</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>1990</v>
+        <v>2020</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -565,10 +565,10 @@
         </is>
       </c>
       <c r="E8">
-        <v>42099.3</v>
+        <v>46124.3</v>
       </c>
       <c r="F8">
-        <v>32.94601427986954</v>
+        <v>16.11395117485444</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>1990</v>
+        <v>2020</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -591,10 +591,10 @@
         </is>
       </c>
       <c r="E9">
-        <v>7881.3</v>
+        <v>21987.453585</v>
       </c>
       <c r="F9">
-        <v>6.167737286461671</v>
+        <v>7.681520446447279</v>
       </c>
     </row>
     <row r="10">
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>1990</v>
+        <v>2020</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="E10">
-        <v>12055</v>
+        <v>28115.1</v>
       </c>
       <c r="F10">
-        <v>9.433985889167452</v>
+        <v>9.822270444779651</v>
       </c>
     </row>
     <row r="11">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>1990</v>
+        <v>2020</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -643,10 +643,10 @@
         </is>
       </c>
       <c r="E11">
-        <v>3055.97</v>
+        <v>98385.54700000001</v>
       </c>
       <c r="F11">
-        <v>2.391536943817425</v>
+        <v>34.37190159350596</v>
       </c>
     </row>
     <row r="12">
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>1990</v>
+        <v>2020</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -669,10 +669,10 @@
         </is>
       </c>
       <c r="E12">
-        <v>41972.39999999999</v>
+        <v>56767.5</v>
       </c>
       <c r="F12">
-        <v>32.84670504641161</v>
+        <v>19.8322516183129</v>
       </c>
     </row>
     <row r="13">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>1990</v>
+        <v>2020</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -695,10 +695,10 @@
         </is>
       </c>
       <c r="E13">
-        <v>20718.71</v>
+        <v>34858.4</v>
       </c>
       <c r="F13">
-        <v>16.2140205542723</v>
+        <v>12.17810472209976</v>
       </c>
     </row>
     <row r="14">
@@ -708,7 +708,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>2005</v>
+        <v>2025</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -721,10 +721,10 @@
         </is>
       </c>
       <c r="E14">
-        <v>59066.3</v>
+        <v>114731</v>
       </c>
       <c r="F14">
-        <v>32.15437111811132</v>
+        <v>30.17082566375258</v>
       </c>
     </row>
     <row r="15">
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>2005</v>
+        <v>2025</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -747,10 +747,10 @@
         </is>
       </c>
       <c r="E15">
-        <v>12630.82</v>
+        <v>20949.259422</v>
       </c>
       <c r="F15">
-        <v>6.875935580966859</v>
+        <v>5.509029414943546</v>
       </c>
     </row>
     <row r="16">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>2005</v>
+        <v>2025</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -773,10 +773,10 @@
         </is>
       </c>
       <c r="E16">
-        <v>17314.4</v>
+        <v>46238.4</v>
       </c>
       <c r="F16">
-        <v>9.425571659092014</v>
+        <v>12.15931792951214</v>
       </c>
     </row>
     <row r="17">
@@ -786,7 +786,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>2005</v>
+        <v>2025</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -799,10 +799,10 @@
         </is>
       </c>
       <c r="E17">
-        <v>6307.87</v>
+        <v>84235.6005</v>
       </c>
       <c r="F17">
-        <v>3.433863183317744</v>
+        <v>22.1514465782309</v>
       </c>
     </row>
     <row r="18">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>2005</v>
+        <v>2025</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -825,10 +825,10 @@
         </is>
       </c>
       <c r="E18">
-        <v>55492.10000000001</v>
+        <v>47264.10000000001</v>
       </c>
       <c r="F18">
-        <v>30.20865667095019</v>
+        <v>12.42904638898091</v>
       </c>
     </row>
     <row r="19">
@@ -838,7 +838,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>2005</v>
+        <v>2025</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -851,10 +851,10 @@
         </is>
       </c>
       <c r="E19">
-        <v>32884.53</v>
+        <v>66852.97</v>
       </c>
       <c r="F19">
-        <v>17.90160178756186</v>
+        <v>17.58033402457994</v>
       </c>
     </row>
     <row r="20">
@@ -864,7 +864,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>2010</v>
+        <v>2030</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -877,10 +877,10 @@
         </is>
       </c>
       <c r="E20">
-        <v>100564</v>
+        <v>131467</v>
       </c>
       <c r="F20">
-        <v>35.60833802497725</v>
+        <v>31.21859179284652</v>
       </c>
     </row>
     <row r="21">
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>2010</v>
+        <v>2030</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -903,10 +903,10 @@
         </is>
       </c>
       <c r="E21">
-        <v>21106.46</v>
+        <v>26097.361312</v>
       </c>
       <c r="F21">
-        <v>7.473509030971931</v>
+        <v>6.197166358628047</v>
       </c>
     </row>
     <row r="22">
@@ -916,7 +916,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>2010</v>
+        <v>2030</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -929,10 +929,10 @@
         </is>
       </c>
       <c r="E22">
-        <v>18662.1</v>
+        <v>85388.10000000001</v>
       </c>
       <c r="F22">
-        <v>6.60799456123392</v>
+        <v>20.27654269030828</v>
       </c>
     </row>
     <row r="23">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>2010</v>
+        <v>2030</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -955,10 +955,10 @@
         </is>
       </c>
       <c r="E23">
-        <v>14415.34</v>
+        <v>63588.7983</v>
       </c>
       <c r="F23">
-        <v>5.104274884302291</v>
+        <v>15.10000788582194</v>
       </c>
     </row>
     <row r="24">
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>2010</v>
+        <v>2030</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -981,10 +981,10 @@
         </is>
       </c>
       <c r="E24">
-        <v>60052.6</v>
+        <v>41908.2</v>
       </c>
       <c r="F24">
-        <v>21.26380494092069</v>
+        <v>9.951660786151434</v>
       </c>
     </row>
     <row r="25">
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>2010</v>
+        <v>2030</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1007,10 +1007,10 @@
         </is>
       </c>
       <c r="E25">
-        <v>67616.5</v>
+        <v>72668.19</v>
       </c>
       <c r="F25">
-        <v>23.94207855759391</v>
+        <v>17.25603048624379</v>
       </c>
     </row>
     <row r="26">
@@ -1020,7 +1020,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>2015</v>
+        <v>2035</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1033,10 +1033,10 @@
         </is>
       </c>
       <c r="E26">
-        <v>85533.39999999999</v>
+        <v>102512</v>
       </c>
       <c r="F26">
-        <v>24.31690424481558</v>
+        <v>23.30372324310405</v>
       </c>
     </row>
     <row r="27">
@@ -1046,7 +1046,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>2015</v>
+        <v>2035</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1059,10 +1059,10 @@
         </is>
       </c>
       <c r="E27">
-        <v>26724.24</v>
+        <v>26864.324885</v>
       </c>
       <c r="F27">
-        <v>7.597626016216711</v>
+        <v>6.106980570400275</v>
       </c>
     </row>
     <row r="28">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>2015</v>
+        <v>2035</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1085,10 +1085,10 @@
         </is>
       </c>
       <c r="E28">
-        <v>37199</v>
+        <v>129024</v>
       </c>
       <c r="F28">
-        <v>10.57557072445261</v>
+        <v>29.33061093060575</v>
       </c>
     </row>
     <row r="29">
@@ -1098,7 +1098,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>2015</v>
+        <v>2035</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1111,10 +1111,10 @@
         </is>
       </c>
       <c r="E29">
-        <v>50716.57</v>
+        <v>69629.2469</v>
       </c>
       <c r="F29">
-        <v>14.41857772888119</v>
+        <v>15.82859274410177</v>
       </c>
     </row>
     <row r="30">
@@ -1124,7 +1124,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>2015</v>
+        <v>2035</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1137,10 +1137,10 @@
         </is>
       </c>
       <c r="E30">
-        <v>92887</v>
+        <v>37997.9</v>
       </c>
       <c r="F30">
-        <v>26.40751197296243</v>
+        <v>8.637940391555556</v>
       </c>
     </row>
     <row r="31">
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>2015</v>
+        <v>2035</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1163,10 +1163,10 @@
         </is>
       </c>
       <c r="E31">
-        <v>58684.4</v>
+        <v>73867.89999999999</v>
       </c>
       <c r="F31">
-        <v>16.68380931267149</v>
+        <v>16.79215212023261</v>
       </c>
     </row>
     <row r="32">
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>2020</v>
+        <v>2040</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1189,10 +1189,10 @@
         </is>
       </c>
       <c r="E32">
-        <v>46124.3</v>
+        <v>69950.60000000001</v>
       </c>
       <c r="F32">
-        <v>16.11395117485444</v>
+        <v>14.94696646733256</v>
       </c>
     </row>
     <row r="33">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B33">
-        <v>2020</v>
+        <v>2040</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1215,10 +1215,10 @@
         </is>
       </c>
       <c r="E33">
-        <v>21987.453585</v>
+        <v>18878.2750951</v>
       </c>
       <c r="F33">
-        <v>7.681520446447279</v>
+        <v>4.033888841661675</v>
       </c>
     </row>
     <row r="34">
@@ -1228,7 +1228,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>2020</v>
+        <v>2040</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1241,10 +1241,10 @@
         </is>
       </c>
       <c r="E34">
-        <v>28115.1</v>
+        <v>185633</v>
       </c>
       <c r="F34">
-        <v>9.822270444779651</v>
+        <v>39.66585313393088</v>
       </c>
     </row>
     <row r="35">
@@ -1254,7 +1254,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>2020</v>
+        <v>2040</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="E35">
-        <v>98385.54700000001</v>
+        <v>88564.976</v>
       </c>
       <c r="F35">
-        <v>34.37190159350596</v>
+        <v>18.92446564364155</v>
       </c>
     </row>
     <row r="36">
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>2020</v>
+        <v>2040</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1293,10 +1293,10 @@
         </is>
       </c>
       <c r="E36">
-        <v>56767.5</v>
+        <v>33345.9</v>
       </c>
       <c r="F36">
-        <v>19.8322516183129</v>
+        <v>7.125314852524851</v>
       </c>
     </row>
     <row r="37">
@@ -1306,7 +1306,7 @@
         </is>
       </c>
       <c r="B37">
-        <v>2020</v>
+        <v>2040</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -1319,10 +1319,10 @@
         </is>
       </c>
       <c r="E37">
-        <v>34858.4</v>
+        <v>71619.2</v>
       </c>
       <c r="F37">
-        <v>12.17810472209976</v>
+        <v>15.30351106090847</v>
       </c>
     </row>
     <row r="38">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B38">
-        <v>2025</v>
+        <v>2045</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1345,10 +1345,10 @@
         </is>
       </c>
       <c r="E38">
-        <v>114730</v>
+        <v>45522.1</v>
       </c>
       <c r="F38">
-        <v>30.17064757926703</v>
+        <v>8.891052575072299</v>
       </c>
     </row>
     <row r="39">
@@ -1358,7 +1358,7 @@
         </is>
       </c>
       <c r="B39">
-        <v>2025</v>
+        <v>2045</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1371,10 +1371,10 @@
         </is>
       </c>
       <c r="E39">
-        <v>20949.279422</v>
+        <v>10061.07692</v>
       </c>
       <c r="F39">
-        <v>5.509050174154563</v>
+        <v>1.965057935762333</v>
       </c>
     </row>
     <row r="40">
@@ -1384,7 +1384,7 @@
         </is>
       </c>
       <c r="B40">
-        <v>2025</v>
+        <v>2045</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -1397,10 +1397,10 @@
         </is>
       </c>
       <c r="E40">
-        <v>46238.3</v>
+        <v>249941</v>
       </c>
       <c r="F40">
-        <v>12.15932584297414</v>
+        <v>48.81669720127466</v>
       </c>
     </row>
     <row r="41">
@@ -1410,7 +1410,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>2025</v>
+        <v>2045</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1423,10 +1423,10 @@
         </is>
       </c>
       <c r="E41">
-        <v>84235.6206</v>
+        <v>110414.52</v>
       </c>
       <c r="F41">
-        <v>22.15151418760085</v>
+        <v>21.5653781871085</v>
       </c>
     </row>
     <row r="42">
@@ -1436,7 +1436,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>2025</v>
+        <v>2045</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1449,10 +1449,10 @@
         </is>
       </c>
       <c r="E42">
-        <v>47264.10000000001</v>
+        <v>28730.1</v>
       </c>
       <c r="F42">
-        <v>12.42908135841746</v>
+        <v>5.611358649690692</v>
       </c>
     </row>
     <row r="43">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>2025</v>
+        <v>2045</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1475,10 +1475,10 @@
         </is>
       </c>
       <c r="E43">
-        <v>66852.96000000001</v>
+        <v>67330.2</v>
       </c>
       <c r="F43">
-        <v>17.58038085758595</v>
+        <v>13.15045545109151</v>
       </c>
     </row>
     <row r="44">
@@ -1488,7 +1488,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1501,10 +1501,10 @@
         </is>
       </c>
       <c r="E44">
-        <v>131468</v>
+        <v>27732.1</v>
       </c>
       <c r="F44">
-        <v>31.21875066769416</v>
+        <v>4.737903703780242</v>
       </c>
     </row>
     <row r="45">
@@ -1514,7 +1514,7 @@
         </is>
       </c>
       <c r="B45">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -1527,10 +1527,10 @@
         </is>
       </c>
       <c r="E45">
-        <v>26097.401312</v>
+        <v>4737.50635</v>
       </c>
       <c r="F45">
-        <v>6.197160256747514</v>
+        <v>0.8093815067141477</v>
       </c>
     </row>
     <row r="46">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="B46">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1553,10 +1553,10 @@
         </is>
       </c>
       <c r="E46">
-        <v>85388.10000000001</v>
+        <v>320735</v>
       </c>
       <c r="F46">
-        <v>20.27649164730684</v>
+        <v>54.79612234313146</v>
       </c>
     </row>
     <row r="47">
@@ -1566,7 +1566,7 @@
         </is>
       </c>
       <c r="B47">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1579,10 +1579,10 @@
         </is>
       </c>
       <c r="E47">
-        <v>63588.8084</v>
+        <v>146050.418005</v>
       </c>
       <c r="F47">
-        <v>15.09997227230486</v>
+        <v>24.95205254576978</v>
       </c>
     </row>
     <row r="48">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B48">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -1605,10 +1605,10 @@
         </is>
       </c>
       <c r="E48">
-        <v>41908.2</v>
+        <v>24348.24</v>
       </c>
       <c r="F48">
-        <v>9.951635734413394</v>
+        <v>4.15978654615158</v>
       </c>
     </row>
     <row r="49">
@@ -1618,7 +1618,7 @@
         </is>
       </c>
       <c r="B49">
-        <v>2030</v>
+        <v>2050</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -1631,10 +1631,10 @@
         </is>
       </c>
       <c r="E49">
-        <v>72668.2</v>
+        <v>61721</v>
       </c>
       <c r="F49">
-        <v>17.25598942153324</v>
+        <v>10.54475335445279</v>
       </c>
     </row>
     <row r="50">
@@ -1644,7 +1644,7 @@
         </is>
       </c>
       <c r="B50">
-        <v>2035</v>
+        <v>2055</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -1657,10 +1657,10 @@
         </is>
       </c>
       <c r="E50">
-        <v>102512</v>
+        <v>18147.9</v>
       </c>
       <c r="F50">
-        <v>23.30366478467111</v>
+        <v>2.8626594768266</v>
       </c>
     </row>
     <row r="51">
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>2035</v>
+        <v>2055</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1683,10 +1683,10 @@
         </is>
       </c>
       <c r="E51">
-        <v>26864.378385</v>
+        <v>2254.2057</v>
       </c>
       <c r="F51">
-        <v>6.106977412718552</v>
+        <v>0.3555796158134847</v>
       </c>
     </row>
     <row r="52">
@@ -1696,7 +1696,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>2035</v>
+        <v>2055</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1709,10 +1709,10 @@
         </is>
       </c>
       <c r="E52">
-        <v>129025</v>
+        <v>344480</v>
       </c>
       <c r="F52">
-        <v>29.33076467966863</v>
+        <v>54.33845990870718</v>
       </c>
     </row>
     <row r="53">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B53">
-        <v>2035</v>
+        <v>2055</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1735,10 +1735,10 @@
         </is>
       </c>
       <c r="E53">
-        <v>69629.1969</v>
+        <v>189453.708195</v>
       </c>
       <c r="F53">
-        <v>15.82854167105764</v>
+        <v>29.88452951494983</v>
       </c>
     </row>
     <row r="54">
@@ -1748,7 +1748,7 @@
         </is>
       </c>
       <c r="B54">
-        <v>2035</v>
+        <v>2055</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1761,10 +1761,10 @@
         </is>
       </c>
       <c r="E54">
-        <v>37997.9</v>
+        <v>21423.54</v>
       </c>
       <c r="F54">
-        <v>8.637918722895412</v>
+        <v>3.379360686810801</v>
       </c>
     </row>
     <row r="55">
@@ -1774,7 +1774,7 @@
         </is>
       </c>
       <c r="B55">
-        <v>2035</v>
+        <v>2055</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1787,10 +1787,10 @@
         </is>
       </c>
       <c r="E55">
-        <v>73868</v>
+        <v>58193.1</v>
       </c>
       <c r="F55">
-        <v>16.79213272898866</v>
+        <v>9.179410796892093</v>
       </c>
     </row>
     <row r="56">
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="B56">
-        <v>2040</v>
+        <v>2060</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1813,10 +1813,10 @@
         </is>
       </c>
       <c r="E56">
-        <v>69950.5</v>
+        <v>12130</v>
       </c>
       <c r="F56">
-        <v>14.94698215135016</v>
+        <v>1.843839015199067</v>
       </c>
     </row>
     <row r="57">
@@ -1826,7 +1826,7 @@
         </is>
       </c>
       <c r="B57">
-        <v>2040</v>
+        <v>2060</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1839,10 +1839,10 @@
         </is>
       </c>
       <c r="E57">
-        <v>18878.3119951</v>
+        <v>1150.480274</v>
       </c>
       <c r="F57">
-        <v>4.033906726018817</v>
+        <v>0.1748804959124578</v>
       </c>
     </row>
     <row r="58">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B58">
-        <v>2040</v>
+        <v>2060</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1865,10 +1865,10 @@
         </is>
       </c>
       <c r="E58">
-        <v>185632</v>
+        <v>343176</v>
       </c>
       <c r="F58">
-        <v>39.66573778199486</v>
+        <v>52.16498745918838</v>
       </c>
     </row>
     <row r="59">
@@ -1878,7 +1878,7 @@
         </is>
       </c>
       <c r="B59">
-        <v>2040</v>
+        <v>2060</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1891,10 +1891,10 @@
         </is>
       </c>
       <c r="E59">
-        <v>88564.97900000001</v>
+        <v>227706.473389</v>
       </c>
       <c r="F59">
-        <v>18.92451319644179</v>
+        <v>34.61286724221157</v>
       </c>
     </row>
     <row r="60">
@@ -1904,7 +1904,7 @@
         </is>
       </c>
       <c r="B60">
-        <v>2040</v>
+        <v>2060</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1917,10 +1917,10 @@
         </is>
       </c>
       <c r="E60">
-        <v>33345.9</v>
+        <v>18952.69</v>
       </c>
       <c r="F60">
-        <v>7.125332515431729</v>
+        <v>2.880932338414939</v>
       </c>
     </row>
     <row r="61">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="B61">
-        <v>2040</v>
+        <v>2060</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1943,10 +1943,10 @@
         </is>
       </c>
       <c r="E61">
-        <v>71619.09999999999</v>
+        <v>54750.89999999999</v>
       </c>
       <c r="F61">
-        <v>15.30352762876265</v>
+        <v>8.322493449073585</v>
       </c>
     </row>
     <row r="62">
@@ -1956,7 +1956,7 @@
         </is>
       </c>
       <c r="B62">
-        <v>2045</v>
+        <v>2065</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1969,10 +1969,10 @@
         </is>
       </c>
       <c r="E62">
-        <v>45522</v>
+        <v>8603.1</v>
       </c>
       <c r="F62">
-        <v>8.89107322821433</v>
+        <v>1.304526494860531</v>
       </c>
     </row>
     <row r="63">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B63">
-        <v>2045</v>
+        <v>2065</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1995,10 +1995,10 @@
         </is>
       </c>
       <c r="E63">
-        <v>10061.09287</v>
+        <v>652.8247388</v>
       </c>
       <c r="F63">
-        <v>1.96506993240708</v>
+        <v>0.0989907322087394</v>
       </c>
     </row>
     <row r="64">
@@ -2008,7 +2008,7 @@
         </is>
       </c>
       <c r="B64">
-        <v>2045</v>
+        <v>2065</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2021,10 +2021,10 @@
         </is>
       </c>
       <c r="E64">
-        <v>249936</v>
+        <v>332634</v>
       </c>
       <c r="F64">
-        <v>48.81594126723292</v>
+        <v>50.43877975281445</v>
       </c>
     </row>
     <row r="65">
@@ -2034,7 +2034,7 @@
         </is>
       </c>
       <c r="B65">
-        <v>2045</v>
+        <v>2065</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2047,10 +2047,10 @@
         </is>
       </c>
       <c r="E65">
-        <v>110417.09</v>
+        <v>248202.9</v>
       </c>
       <c r="F65">
-        <v>21.56597761162366</v>
+        <v>37.63611479015924</v>
       </c>
     </row>
     <row r="66">
@@ -2060,7 +2060,7 @@
         </is>
       </c>
       <c r="B66">
-        <v>2045</v>
+        <v>2065</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2073,10 +2073,10 @@
         </is>
       </c>
       <c r="E66">
-        <v>28730.2</v>
+        <v>17121.64</v>
       </c>
       <c r="F66">
-        <v>5.611403542490299</v>
+        <v>2.596230779075434</v>
       </c>
     </row>
     <row r="67">
@@ -2086,7 +2086,7 @@
         </is>
       </c>
       <c r="B67">
-        <v>2045</v>
+        <v>2065</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2099,10 +2099,10 @@
         </is>
       </c>
       <c r="E67">
-        <v>67330.3</v>
+        <v>52266.2</v>
       </c>
       <c r="F67">
-        <v>13.15053441803171</v>
+        <v>7.925357450881601</v>
       </c>
     </row>
     <row r="68">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="B68">
-        <v>2050</v>
+        <v>2070</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2125,10 +2125,10 @@
         </is>
       </c>
       <c r="E68">
-        <v>27742.6</v>
+        <v>6567.59</v>
       </c>
       <c r="F68">
-        <v>4.740999007000616</v>
+        <v>1.023531497640096</v>
       </c>
     </row>
     <row r="69">
@@ -2138,7 +2138,7 @@
         </is>
       </c>
       <c r="B69">
-        <v>2050</v>
+        <v>2070</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2151,10 +2151,10 @@
         </is>
       </c>
       <c r="E69">
-        <v>4737.73865</v>
+        <v>410.4443</v>
       </c>
       <c r="F69">
-        <v>0.8096434449214722</v>
+        <v>0.06396603153924665</v>
       </c>
     </row>
     <row r="70">
@@ -2164,7 +2164,7 @@
         </is>
       </c>
       <c r="B70">
-        <v>2050</v>
+        <v>2070</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2177,10 +2177,10 @@
         </is>
       </c>
       <c r="E70">
-        <v>320547</v>
+        <v>322738</v>
       </c>
       <c r="F70">
-        <v>54.77904048996945</v>
+        <v>50.2973706466709</v>
       </c>
     </row>
     <row r="71">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="B71">
-        <v>2050</v>
+        <v>2070</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2203,10 +2203,10 @@
         </is>
       </c>
       <c r="E71">
-        <v>146072.921535</v>
+        <v>245600</v>
       </c>
       <c r="F71">
-        <v>24.96274956013906</v>
+        <v>38.27573521191299</v>
       </c>
     </row>
     <row r="72">
@@ -2216,7 +2216,7 @@
         </is>
       </c>
       <c r="B72">
-        <v>2050</v>
+        <v>2070</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2229,10 +2229,10 @@
         </is>
       </c>
       <c r="E72">
-        <v>24346.73</v>
+        <v>15762.55</v>
       </c>
       <c r="F72">
-        <v>4.160670692498615</v>
+        <v>2.456527646842586</v>
       </c>
     </row>
     <row r="73">
@@ -2242,7 +2242,7 @@
         </is>
       </c>
       <c r="B73">
-        <v>2050</v>
+        <v>2070</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2255,20 +2255,20 @@
         </is>
       </c>
       <c r="E73">
-        <v>61716.60000000001</v>
+        <v>50581.2</v>
       </c>
       <c r="F73">
-        <v>10.5468968054708</v>
+        <v>7.88286896539419</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B74">
-        <v>2055</v>
+        <v>2015</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2281,20 +2281,20 @@
         </is>
       </c>
       <c r="E74">
-        <v>18147</v>
+        <v>85533.39999999999</v>
       </c>
       <c r="F74">
-        <v>2.862529445201077</v>
+        <v>24.31690424481558</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B75">
-        <v>2055</v>
+        <v>2015</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -2307,20 +2307,20 @@
         </is>
       </c>
       <c r="E75">
-        <v>2254.39708</v>
+        <v>26724.24</v>
       </c>
       <c r="F75">
-        <v>0.3556112868614828</v>
+        <v>7.597626016216711</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B76">
-        <v>2055</v>
+        <v>2015</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -2333,20 +2333,20 @@
         </is>
       </c>
       <c r="E76">
-        <v>344463</v>
+        <v>37199</v>
       </c>
       <c r="F76">
-        <v>54.3360048648426</v>
+        <v>10.57557072445261</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B77">
-        <v>2055</v>
+        <v>2015</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2359,20 +2359,20 @@
         </is>
       </c>
       <c r="E77">
-        <v>189469.303652</v>
+        <v>50716.57</v>
       </c>
       <c r="F77">
-        <v>29.8871141602245</v>
+        <v>14.41857772888119</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B78">
-        <v>2055</v>
+        <v>2015</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2385,20 +2385,20 @@
         </is>
       </c>
       <c r="E78">
-        <v>21423.41</v>
+        <v>92887</v>
       </c>
       <c r="F78">
-        <v>3.3793542702163</v>
+        <v>26.40751197296243</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B79">
-        <v>2055</v>
+        <v>2015</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2411,20 +2411,20 @@
         </is>
       </c>
       <c r="E79">
-        <v>58192.7</v>
+        <v>58684.4</v>
       </c>
       <c r="F79">
-        <v>9.179385972654032</v>
+        <v>16.68380931267149</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B80">
-        <v>2060</v>
+        <v>2020</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2437,20 +2437,20 @@
         </is>
       </c>
       <c r="E80">
-        <v>12129.9</v>
+        <v>46124.3</v>
       </c>
       <c r="F80">
-        <v>1.843822589933835</v>
+        <v>16.11395117485444</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B81">
-        <v>2060</v>
+        <v>2020</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2463,20 +2463,20 @@
         </is>
       </c>
       <c r="E81">
-        <v>1150.613718</v>
+        <v>21987.453585</v>
       </c>
       <c r="F81">
-        <v>0.1749006641057354</v>
+        <v>7.681520446447279</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B82">
-        <v>2060</v>
+        <v>2020</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2489,20 +2489,20 @@
         </is>
       </c>
       <c r="E82">
-        <v>343175</v>
+        <v>28115.1</v>
       </c>
       <c r="F82">
-        <v>52.16480080631693</v>
+        <v>9.822270444779651</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B83">
-        <v>2060</v>
+        <v>2020</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -2515,20 +2515,20 @@
         </is>
       </c>
       <c r="E83">
-        <v>227707.776881</v>
+        <v>98385.54700000001</v>
       </c>
       <c r="F83">
-        <v>34.61304239250128</v>
+        <v>34.37190159350596</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B84">
-        <v>2060</v>
+        <v>2020</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -2541,20 +2541,20 @@
         </is>
       </c>
       <c r="E84">
-        <v>18952.69</v>
+        <v>56767.5</v>
       </c>
       <c r="F84">
-        <v>2.880930424983973</v>
+        <v>19.8322516183129</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B85">
-        <v>2060</v>
+        <v>2020</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2567,20 +2567,20 @@
         </is>
       </c>
       <c r="E85">
-        <v>54751</v>
+        <v>34858.4</v>
       </c>
       <c r="F85">
-        <v>8.322503122158253</v>
+        <v>12.17810472209976</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B86">
-        <v>2065</v>
+        <v>2025</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2593,20 +2593,20 @@
         </is>
       </c>
       <c r="E86">
-        <v>8603.129999999999</v>
+        <v>114732</v>
       </c>
       <c r="F86">
-        <v>1.304531523790315</v>
+        <v>30.17104349688076</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B87">
-        <v>2065</v>
+        <v>2025</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2619,20 +2619,20 @@
         </is>
       </c>
       <c r="E87">
-        <v>652.8521368</v>
+        <v>20948.829422</v>
       </c>
       <c r="F87">
-        <v>0.09899492310699332</v>
+        <v>5.508908096258213</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B88">
-        <v>2065</v>
+        <v>2025</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2645,20 +2645,20 @@
         </is>
       </c>
       <c r="E88">
-        <v>332635</v>
+        <v>46238.6</v>
       </c>
       <c r="F88">
-        <v>50.43894994217122</v>
+        <v>12.15935233269594</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B89">
-        <v>2065</v>
+        <v>2025</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -2671,20 +2671,20 @@
         </is>
       </c>
       <c r="E89">
-        <v>248201.6</v>
+        <v>84235.53939999999</v>
       </c>
       <c r="F89">
-        <v>37.63593151041474</v>
+        <v>22.15139737144487</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B90">
-        <v>2065</v>
+        <v>2025</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -2697,20 +2697,20 @@
         </is>
       </c>
       <c r="E90">
-        <v>17121.64</v>
+        <v>47264</v>
       </c>
       <c r="F90">
-        <v>2.596231734146667</v>
+        <v>12.4290014977214</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B91">
-        <v>2065</v>
+        <v>2025</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -2723,20 +2723,20 @@
         </is>
       </c>
       <c r="E91">
-        <v>52266.2</v>
+        <v>66852.93000000001</v>
       </c>
       <c r="F91">
-        <v>7.925360366370073</v>
+        <v>17.58029720499882</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B92">
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -2749,20 +2749,20 @@
         </is>
       </c>
       <c r="E92">
-        <v>6567.58</v>
+        <v>131468</v>
       </c>
       <c r="F92">
-        <v>1.023530433512446</v>
+        <v>31.21875593854415</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B93">
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2775,20 +2775,20 @@
         </is>
       </c>
       <c r="E93">
-        <v>410.4444</v>
+        <v>26097.011312</v>
       </c>
       <c r="F93">
-        <v>0.06396607801728425</v>
+        <v>6.197068692569704</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B94">
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2801,20 +2801,20 @@
         </is>
       </c>
       <c r="E94">
-        <v>322738</v>
+        <v>85388.5</v>
       </c>
       <c r="F94">
-        <v>50.29739493861357</v>
+        <v>20.27659005581873</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B95">
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2827,20 +2827,20 @@
         </is>
       </c>
       <c r="E95">
-        <v>245599.9</v>
+        <v>63588.5773</v>
       </c>
       <c r="F95">
-        <v>38.27573811321877</v>
+        <v>15.09991994407725</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B96">
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -2853,20 +2853,20 @@
         </is>
       </c>
       <c r="E96">
-        <v>15762.55</v>
+        <v>41908.1</v>
       </c>
       <c r="F96">
-        <v>2.456528833263028</v>
+        <v>9.951613668330712</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Net_Zero</t>
+          <t>Reference</t>
         </is>
       </c>
       <c r="B97">
-        <v>2070</v>
+        <v>2030</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -2879,10 +2879,10 @@
         </is>
       </c>
       <c r="E97">
-        <v>50581</v>
+        <v>72668.45</v>
       </c>
       <c r="F97">
-        <v>7.882841603374915</v>
+        <v>17.25605170065946</v>
       </c>
     </row>
     <row r="98">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="B98">
-        <v>1975</v>
+        <v>2035</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -2905,10 +2905,10 @@
         </is>
       </c>
       <c r="E98">
-        <v>14116.1</v>
+        <v>102393</v>
       </c>
       <c r="F98">
-        <v>23.72764633618808</v>
+        <v>23.29161973474793</v>
       </c>
     </row>
     <row r="99">
@@ -2918,7 +2918,7 @@
         </is>
       </c>
       <c r="B99">
-        <v>1975</v>
+        <v>2035</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -2931,10 +2931,10 @@
         </is>
       </c>
       <c r="E99">
-        <v>2682.94</v>
+        <v>26840.563785</v>
       </c>
       <c r="F99">
-        <v>4.509733670150569</v>
+        <v>6.105497496376378</v>
       </c>
     </row>
     <row r="100">
@@ -2944,7 +2944,7 @@
         </is>
       </c>
       <c r="B100">
-        <v>1975</v>
+        <v>2035</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -2957,10 +2957,10 @@
         </is>
       </c>
       <c r="E100">
-        <v>4082.4</v>
+        <v>128952</v>
       </c>
       <c r="F100">
-        <v>6.862075460138013</v>
+        <v>29.33306913592936</v>
       </c>
     </row>
     <row r="101">
@@ -2970,7 +2970,7 @@
         </is>
       </c>
       <c r="B101">
-        <v>1975</v>
+        <v>2035</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -2983,10 +2983,10 @@
         </is>
       </c>
       <c r="E101">
-        <v>998.735</v>
+        <v>69645.9866</v>
       </c>
       <c r="F101">
-        <v>1.67876615096045</v>
+        <v>15.8425657607312</v>
       </c>
     </row>
     <row r="102">
@@ -2996,7 +2996,7 @@
         </is>
       </c>
       <c r="B102">
-        <v>1975</v>
+        <v>2035</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -3009,10 +3009,10 @@
         </is>
       </c>
       <c r="E102">
-        <v>30093.7</v>
+        <v>38005.8</v>
       </c>
       <c r="F102">
-        <v>50.58427402379858</v>
+        <v>8.645284749102798</v>
       </c>
     </row>
     <row r="103">
@@ -3022,7 +3022,7 @@
         </is>
       </c>
       <c r="B103">
-        <v>1975</v>
+        <v>2035</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -3035,10 +3035,10 @@
         </is>
       </c>
       <c r="E103">
-        <v>7518.33</v>
+        <v>73775.7</v>
       </c>
       <c r="F103">
-        <v>12.63750435876431</v>
+        <v>16.78196312311235</v>
       </c>
     </row>
     <row r="104">
@@ -3048,7 +3048,7 @@
         </is>
       </c>
       <c r="B104">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -3061,10 +3061,10 @@
         </is>
       </c>
       <c r="E104">
-        <v>42099.3</v>
+        <v>69918.5</v>
       </c>
       <c r="F104">
-        <v>32.94601427986954</v>
+        <v>14.94636499230888</v>
       </c>
     </row>
     <row r="105">
@@ -3074,7 +3074,7 @@
         </is>
       </c>
       <c r="B105">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -3087,10 +3087,10 @@
         </is>
       </c>
       <c r="E105">
-        <v>7881.3</v>
+        <v>18850.9361951</v>
       </c>
       <c r="F105">
-        <v>6.167737286461671</v>
+        <v>4.029734230835773</v>
       </c>
     </row>
     <row r="106">
@@ -3100,7 +3100,7 @@
         </is>
       </c>
       <c r="B106">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -3113,10 +3113,10 @@
         </is>
       </c>
       <c r="E106">
-        <v>12055</v>
+        <v>185540</v>
       </c>
       <c r="F106">
-        <v>9.433985889167452</v>
+        <v>39.66258659257549</v>
       </c>
     </row>
     <row r="107">
@@ -3126,7 +3126,7 @@
         </is>
       </c>
       <c r="B107">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -3139,10 +3139,10 @@
         </is>
       </c>
       <c r="E107">
-        <v>3055.97</v>
+        <v>88578.08</v>
       </c>
       <c r="F107">
-        <v>2.391536943817425</v>
+        <v>18.93519331790492</v>
       </c>
     </row>
     <row r="108">
@@ -3152,7 +3152,7 @@
         </is>
       </c>
       <c r="B108">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -3165,10 +3165,10 @@
         </is>
       </c>
       <c r="E108">
-        <v>41972.39999999999</v>
+        <v>33350.3</v>
       </c>
       <c r="F108">
-        <v>32.84670504641161</v>
+        <v>7.12923984929595</v>
       </c>
     </row>
     <row r="109">
@@ -3178,7 +3178,7 @@
         </is>
       </c>
       <c r="B109">
-        <v>1990</v>
+        <v>2040</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -3191,10 +3191,10 @@
         </is>
       </c>
       <c r="E109">
-        <v>20718.71</v>
+        <v>71558.2</v>
       </c>
       <c r="F109">
-        <v>16.2140205542723</v>
+        <v>15.29688101707899</v>
       </c>
     </row>
     <row r="110">
@@ -3204,7 +3204,7 @@
         </is>
       </c>
       <c r="B110">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -3217,10 +3217,10 @@
         </is>
       </c>
       <c r="E110">
-        <v>59066.3</v>
+        <v>45509.3</v>
       </c>
       <c r="F110">
-        <v>32.15437111811132</v>
+        <v>8.895124424150811</v>
       </c>
     </row>
     <row r="111">
@@ -3230,7 +3230,7 @@
         </is>
       </c>
       <c r="B111">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -3243,10 +3243,10 @@
         </is>
       </c>
       <c r="E111">
-        <v>12630.82</v>
+        <v>10040.91423</v>
       </c>
       <c r="F111">
-        <v>6.875935580966859</v>
+        <v>1.962569879301076</v>
       </c>
     </row>
     <row r="112">
@@ -3256,7 +3256,7 @@
         </is>
       </c>
       <c r="B112">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -3269,10 +3269,10 @@
         </is>
       </c>
       <c r="E112">
-        <v>17314.4</v>
+        <v>249237</v>
       </c>
       <c r="F112">
-        <v>9.425571659092014</v>
+        <v>48.71518845822889</v>
       </c>
     </row>
     <row r="113">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="B113">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -3295,10 +3295,10 @@
         </is>
       </c>
       <c r="E113">
-        <v>6307.87</v>
+        <v>110777.91</v>
       </c>
       <c r="F113">
-        <v>3.433863183317744</v>
+        <v>21.65235002290478</v>
       </c>
     </row>
     <row r="114">
@@ -3308,7 +3308,7 @@
         </is>
       </c>
       <c r="B114">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -3321,10 +3321,10 @@
         </is>
       </c>
       <c r="E114">
-        <v>55492.10000000001</v>
+        <v>28740.1</v>
       </c>
       <c r="F114">
-        <v>30.20865667095019</v>
+        <v>5.617462045395924</v>
       </c>
     </row>
     <row r="115">
@@ -3334,7 +3334,7 @@
         </is>
       </c>
       <c r="B115">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -3347,10 +3347,10 @@
         </is>
       </c>
       <c r="E115">
-        <v>32884.53</v>
+        <v>67315.5</v>
       </c>
       <c r="F115">
-        <v>17.90160178756186</v>
+        <v>13.15730517001853</v>
       </c>
     </row>
     <row r="116">
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="B116">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -3373,10 +3373,10 @@
         </is>
       </c>
       <c r="E116">
-        <v>100564</v>
+        <v>29343.2</v>
       </c>
       <c r="F116">
-        <v>35.60833802497725</v>
+        <v>5.140637699304518</v>
       </c>
     </row>
     <row r="117">
@@ -3386,7 +3386,7 @@
         </is>
       </c>
       <c r="B117">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -3399,10 +3399,10 @@
         </is>
       </c>
       <c r="E117">
-        <v>21106.46</v>
+        <v>4771.63949</v>
       </c>
       <c r="F117">
-        <v>7.473509030971931</v>
+        <v>0.8359439273761615</v>
       </c>
     </row>
     <row r="118">
@@ -3412,7 +3412,7 @@
         </is>
       </c>
       <c r="B118">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -3425,10 +3425,10 @@
         </is>
       </c>
       <c r="E118">
-        <v>18662.1</v>
+        <v>299906</v>
       </c>
       <c r="F118">
-        <v>6.60799456123392</v>
+        <v>52.54055760270254</v>
       </c>
     </row>
     <row r="119">
@@ -3438,7 +3438,7 @@
         </is>
       </c>
       <c r="B119">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -3451,10 +3451,10 @@
         </is>
       </c>
       <c r="E119">
-        <v>14415.34</v>
+        <v>150160.74</v>
       </c>
       <c r="F119">
-        <v>5.104274884302291</v>
+        <v>26.30667278958886</v>
       </c>
     </row>
     <row r="120">
@@ -3464,7 +3464,7 @@
         </is>
       </c>
       <c r="B120">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -3477,10 +3477,10 @@
         </is>
       </c>
       <c r="E120">
-        <v>60052.6</v>
+        <v>24527.68</v>
       </c>
       <c r="F120">
-        <v>21.26380494092069</v>
+        <v>4.297006341655902</v>
       </c>
     </row>
     <row r="121">
@@ -3490,7 +3490,7 @@
         </is>
       </c>
       <c r="B121">
-        <v>2010</v>
+        <v>2050</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -3503,10 +3503,10 @@
         </is>
       </c>
       <c r="E121">
-        <v>67616.5</v>
+        <v>62099.3</v>
       </c>
       <c r="F121">
-        <v>23.94207855759391</v>
+        <v>10.87918163937202</v>
       </c>
     </row>
     <row r="122">
@@ -3516,7 +3516,7 @@
         </is>
       </c>
       <c r="B122">
-        <v>2015</v>
+        <v>2055</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -3529,10 +3529,10 @@
         </is>
       </c>
       <c r="E122">
-        <v>85533.39999999999</v>
+        <v>18031</v>
       </c>
       <c r="F122">
-        <v>24.31690424481558</v>
+        <v>2.905397864713245</v>
       </c>
     </row>
     <row r="123">
@@ -3542,7 +3542,7 @@
         </is>
       </c>
       <c r="B123">
-        <v>2015</v>
+        <v>2055</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -3555,10 +3555,10 @@
         </is>
       </c>
       <c r="E123">
-        <v>26724.24</v>
+        <v>2294.34118</v>
       </c>
       <c r="F123">
-        <v>7.597626016216711</v>
+        <v>0.3696951896897381</v>
       </c>
     </row>
     <row r="124">
@@ -3568,7 +3568,7 @@
         </is>
       </c>
       <c r="B124">
-        <v>2015</v>
+        <v>2055</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -3581,10 +3581,10 @@
         </is>
       </c>
       <c r="E124">
-        <v>37199</v>
+        <v>328577</v>
       </c>
       <c r="F124">
-        <v>10.57557072445261</v>
+        <v>52.94475704031301</v>
       </c>
     </row>
     <row r="125">
@@ -3594,7 +3594,7 @@
         </is>
       </c>
       <c r="B125">
-        <v>2015</v>
+        <v>2055</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -3607,10 +3607,10 @@
         </is>
       </c>
       <c r="E125">
-        <v>50716.57</v>
+        <v>192638.93</v>
       </c>
       <c r="F125">
-        <v>14.41857772888119</v>
+        <v>31.04058210208221</v>
       </c>
     </row>
     <row r="126">
@@ -3620,7 +3620,7 @@
         </is>
       </c>
       <c r="B126">
-        <v>2015</v>
+        <v>2055</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -3633,10 +3633,10 @@
         </is>
       </c>
       <c r="E126">
-        <v>92887</v>
+        <v>21297.9</v>
       </c>
       <c r="F126">
-        <v>26.40751197296243</v>
+        <v>3.431804846257902</v>
       </c>
     </row>
     <row r="127">
@@ -3646,7 +3646,7 @@
         </is>
       </c>
       <c r="B127">
-        <v>2015</v>
+        <v>2055</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -3659,10 +3659,10 @@
         </is>
       </c>
       <c r="E127">
-        <v>58684.4</v>
+        <v>57764.3</v>
       </c>
       <c r="F127">
-        <v>16.68380931267149</v>
+        <v>9.307762956943892</v>
       </c>
     </row>
     <row r="128">
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="B128">
-        <v>2020</v>
+        <v>2060</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -3685,10 +3685,10 @@
         </is>
       </c>
       <c r="E128">
-        <v>46124.3</v>
+        <v>12112.9</v>
       </c>
       <c r="F128">
-        <v>16.11395117485444</v>
+        <v>1.879924919255779</v>
       </c>
     </row>
     <row r="129">
@@ -3698,7 +3698,7 @@
         </is>
       </c>
       <c r="B129">
-        <v>2020</v>
+        <v>2060</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -3711,10 +3711,10 @@
         </is>
       </c>
       <c r="E129">
-        <v>21987.453585</v>
+        <v>1182.473774</v>
       </c>
       <c r="F129">
-        <v>7.681520446447279</v>
+        <v>0.1835202068958735</v>
       </c>
     </row>
     <row r="130">
@@ -3724,7 +3724,7 @@
         </is>
       </c>
       <c r="B130">
-        <v>2020</v>
+        <v>2060</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -3737,10 +3737,10 @@
         </is>
       </c>
       <c r="E130">
-        <v>28115.1</v>
+        <v>329772</v>
       </c>
       <c r="F130">
-        <v>9.822270444779651</v>
+        <v>51.18069169833952</v>
       </c>
     </row>
     <row r="131">
@@ -3750,7 +3750,7 @@
         </is>
       </c>
       <c r="B131">
-        <v>2020</v>
+        <v>2060</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -3763,10 +3763,10 @@
         </is>
       </c>
       <c r="E131">
-        <v>98385.54700000001</v>
+        <v>228136.21</v>
       </c>
       <c r="F131">
-        <v>34.37190159350596</v>
+        <v>35.40679326697731</v>
       </c>
     </row>
     <row r="132">
@@ -3776,7 +3776,7 @@
         </is>
       </c>
       <c r="B132">
-        <v>2020</v>
+        <v>2060</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -3789,10 +3789,10 @@
         </is>
       </c>
       <c r="E132">
-        <v>56767.5</v>
+        <v>18820.74</v>
       </c>
       <c r="F132">
-        <v>19.8322516183129</v>
+        <v>2.920983259569055</v>
       </c>
     </row>
     <row r="133">
@@ -3802,7 +3802,7 @@
         </is>
       </c>
       <c r="B133">
-        <v>2020</v>
+        <v>2060</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -3815,10 +3815,10 @@
         </is>
       </c>
       <c r="E133">
-        <v>34858.4</v>
+        <v>54304.60000000001</v>
       </c>
       <c r="F133">
-        <v>12.17810472209976</v>
+        <v>8.428086648962459</v>
       </c>
     </row>
     <row r="134">
@@ -3828,7 +3828,7 @@
         </is>
       </c>
       <c r="B134">
-        <v>2025</v>
+        <v>2065</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -3841,10 +3841,10 @@
         </is>
       </c>
       <c r="E134">
-        <v>114732</v>
+        <v>8590.48</v>
       </c>
       <c r="F134">
-        <v>30.17104190213252</v>
+        <v>1.328807643686627</v>
       </c>
     </row>
     <row r="135">
@@ -3854,7 +3854,7 @@
         </is>
       </c>
       <c r="B135">
-        <v>2025</v>
+        <v>2065</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -3867,10 +3867,10 @@
         </is>
       </c>
       <c r="E135">
-        <v>20948.859422</v>
+        <v>663.0469920000001</v>
       </c>
       <c r="F135">
-        <v>5.508915694165931</v>
+        <v>0.1025625938356211</v>
       </c>
     </row>
     <row r="136">
@@ -3880,7 +3880,7 @@
         </is>
       </c>
       <c r="B136">
-        <v>2025</v>
+        <v>2065</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -3893,10 +3893,10 @@
         </is>
       </c>
       <c r="E136">
-        <v>46238.6</v>
+        <v>320581</v>
       </c>
       <c r="F136">
-        <v>12.1593516899901</v>
+        <v>49.58867062384206</v>
       </c>
     </row>
     <row r="137">
@@ -3906,7 +3906,7 @@
         </is>
       </c>
       <c r="B137">
-        <v>2025</v>
+        <v>2065</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -3919,10 +3919,10 @@
         </is>
       </c>
       <c r="E137">
-        <v>84235.5395</v>
+        <v>247826.05</v>
       </c>
       <c r="F137">
-        <v>22.15139622688734</v>
+        <v>38.33466227087012</v>
       </c>
     </row>
     <row r="138">
@@ -3932,7 +3932,7 @@
         </is>
       </c>
       <c r="B138">
-        <v>2025</v>
+        <v>2065</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -3945,10 +3945,10 @@
         </is>
       </c>
       <c r="E138">
-        <v>47264</v>
+        <v>16995.65</v>
       </c>
       <c r="F138">
-        <v>12.42900084076274</v>
+        <v>2.628950842027761</v>
       </c>
     </row>
     <row r="139">
@@ -3958,7 +3958,7 @@
         </is>
       </c>
       <c r="B139">
-        <v>2025</v>
+        <v>2065</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -3971,10 +3971,10 @@
         </is>
       </c>
       <c r="E139">
-        <v>66852.92</v>
+        <v>51824.1</v>
       </c>
       <c r="F139">
-        <v>17.58029364606137</v>
+        <v>8.016346025737811</v>
       </c>
     </row>
     <row r="140">
@@ -3984,7 +3984,7 @@
         </is>
       </c>
       <c r="B140">
-        <v>2030</v>
+        <v>2070</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -3997,10 +3997,10 @@
         </is>
       </c>
       <c r="E140">
-        <v>131468</v>
+        <v>6549.88</v>
       </c>
       <c r="F140">
-        <v>31.21875296581418</v>
+        <v>1.040166075899329</v>
       </c>
     </row>
     <row r="141">
@@ -4010,7 +4010,7 @@
         </is>
       </c>
       <c r="B141">
-        <v>2030</v>
+        <v>2070</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -4023,10 +4023,10 @@
         </is>
       </c>
       <c r="E141">
-        <v>26097.041312</v>
+        <v>413.0187857</v>
       </c>
       <c r="F141">
-        <v>6.197075226351472</v>
+        <v>0.06559022907202497</v>
       </c>
     </row>
     <row r="142">
@@ -4036,7 +4036,7 @@
         </is>
       </c>
       <c r="B142">
-        <v>2030</v>
+        <v>2070</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -4049,10 +4049,10 @@
         </is>
       </c>
       <c r="E142">
-        <v>85388.5</v>
+        <v>311704</v>
       </c>
       <c r="F142">
-        <v>20.27658812502985</v>
+        <v>49.50074299408913</v>
       </c>
     </row>
     <row r="143">
@@ -4062,7 +4062,7 @@
         </is>
       </c>
       <c r="B143">
-        <v>2030</v>
+        <v>2070</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
@@ -4075,10 +4075,10 @@
         </is>
       </c>
       <c r="E143">
-        <v>63588.5774</v>
+        <v>245214.31</v>
       </c>
       <c r="F143">
-        <v>15.09991852997045</v>
+        <v>38.94172207537567</v>
       </c>
     </row>
     <row r="144">
@@ -4088,7 +4088,7 @@
         </is>
       </c>
       <c r="B144">
-        <v>2030</v>
+        <v>2070</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
@@ -4101,10 +4101,10 @@
         </is>
       </c>
       <c r="E144">
-        <v>41908.1</v>
+        <v>15646.69</v>
       </c>
       <c r="F144">
-        <v>9.951612720712548</v>
+        <v>2.484802185400843</v>
       </c>
     </row>
     <row r="145">
@@ -4114,7 +4114,7 @@
         </is>
       </c>
       <c r="B145">
-        <v>2030</v>
+        <v>2070</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
@@ -4127,1258 +4127,10 @@
         </is>
       </c>
       <c r="E145">
-        <v>72668.46000000001</v>
+        <v>50167.7</v>
       </c>
       <c r="F145">
-        <v>17.2560524321215</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B146">
-        <v>2035</v>
-      </c>
-      <c r="C146" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D146" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E146">
-        <v>102393</v>
-      </c>
-      <c r="F146">
-        <v>23.29162299844534</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B147">
-        <v>2035</v>
-      </c>
-      <c r="C147" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D147" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E147">
-        <v>26840.582185</v>
-      </c>
-      <c r="F147">
-        <v>6.105502537398146</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B148">
-        <v>2035</v>
-      </c>
-      <c r="C148" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D148" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E148">
-        <v>128952</v>
-      </c>
-      <c r="F148">
-        <v>29.33307324617428</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B149">
-        <v>2035</v>
-      </c>
-      <c r="C149" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D149" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E149">
-        <v>69645.9066</v>
-      </c>
-      <c r="F149">
-        <v>15.84254978281852</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B150">
-        <v>2035</v>
-      </c>
-      <c r="C150" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D150" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E150">
-        <v>38005.8</v>
-      </c>
-      <c r="F150">
-        <v>8.645285960508179</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B151">
-        <v>2035</v>
-      </c>
-      <c r="C151" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D151" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E151">
-        <v>73775.7</v>
-      </c>
-      <c r="F151">
-        <v>16.78196547465553</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B152">
-        <v>2040</v>
-      </c>
-      <c r="C152" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D152" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E152">
-        <v>69918.39999999999</v>
-      </c>
-      <c r="F152">
-        <v>14.94634389663506</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B153">
-        <v>2040</v>
-      </c>
-      <c r="C153" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D153" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E153">
-        <v>18850.9263951</v>
-      </c>
-      <c r="F153">
-        <v>4.02973221171136</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B154">
-        <v>2040</v>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D154" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E154">
-        <v>185540</v>
-      </c>
-      <c r="F154">
-        <v>39.66258733869294</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B155">
-        <v>2040</v>
-      </c>
-      <c r="C155" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D155" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E155">
-        <v>88578.181</v>
-      </c>
-      <c r="F155">
-        <v>18.93521526471409</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B156">
-        <v>2040</v>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E156">
-        <v>33350.3</v>
-      </c>
-      <c r="F156">
-        <v>7.129239983408491</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B157">
-        <v>2040</v>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E157">
-        <v>71558.2</v>
-      </c>
-      <c r="F157">
-        <v>15.29688130483808</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B158">
-        <v>2045</v>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E158">
-        <v>45509.3</v>
-      </c>
-      <c r="F158">
-        <v>8.895137025142438</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B159">
-        <v>2045</v>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E159">
-        <v>10040.90946</v>
-      </c>
-      <c r="F159">
-        <v>1.962571727179916</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B160">
-        <v>2045</v>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E160">
-        <v>249236</v>
-      </c>
-      <c r="F160">
-        <v>48.7150620114658</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B161">
-        <v>2045</v>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E161">
-        <v>110778.19</v>
-      </c>
-      <c r="F161">
-        <v>21.6524354241279</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B162">
-        <v>2045</v>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E162">
-        <v>28740.1</v>
-      </c>
-      <c r="F162">
-        <v>5.617470003192669</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B163">
-        <v>2045</v>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E163">
-        <v>67315.5</v>
-      </c>
-      <c r="F163">
-        <v>13.15732380889127</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B164">
-        <v>2050</v>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E164">
-        <v>29343.2</v>
-      </c>
-      <c r="F164">
-        <v>5.140644685090925</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B165">
-        <v>2050</v>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E165">
-        <v>4771.6338</v>
-      </c>
-      <c r="F165">
-        <v>0.8359440665356953</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B166">
-        <v>2050</v>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E166">
-        <v>299905</v>
-      </c>
-      <c r="F166">
-        <v>52.54045381152002</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B167">
-        <v>2050</v>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E167">
-        <v>150161.17</v>
-      </c>
-      <c r="F167">
-        <v>26.30678387045499</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B168">
-        <v>2050</v>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E168">
-        <v>24527.68</v>
-      </c>
-      <c r="F168">
-        <v>4.297012181003129</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B169">
-        <v>2050</v>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E169">
-        <v>62099.1</v>
-      </c>
-      <c r="F169">
-        <v>10.87916138539525</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B170">
-        <v>2055</v>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E170">
-        <v>18030.9</v>
-      </c>
-      <c r="F170">
-        <v>2.90538063238282</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B171">
-        <v>2055</v>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E171">
-        <v>2294.3402</v>
-      </c>
-      <c r="F171">
-        <v>0.3696948893941692</v>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B172">
-        <v>2055</v>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E172">
-        <v>328577</v>
-      </c>
-      <c r="F172">
-        <v>52.94473664911068</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B173">
-        <v>2055</v>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E173">
-        <v>192639.27</v>
-      </c>
-      <c r="F173">
-        <v>31.04062493244179</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B174">
-        <v>2055</v>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E174">
-        <v>21297.9</v>
-      </c>
-      <c r="F174">
-        <v>3.431803524528784</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B175">
-        <v>2055</v>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E175">
-        <v>57764.3</v>
-      </c>
-      <c r="F175">
-        <v>9.307759372141764</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B176">
-        <v>2060</v>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E176">
-        <v>12112.9</v>
-      </c>
-      <c r="F176">
-        <v>1.8799262029021</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B177">
-        <v>2060</v>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E177">
-        <v>1182.473815</v>
-      </c>
-      <c r="F177">
-        <v>0.1835203385699634</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B178">
-        <v>2060</v>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E178">
-        <v>329771</v>
-      </c>
-      <c r="F178">
-        <v>51.1805714450898</v>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B179">
-        <v>2060</v>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E179">
-        <v>228136.67</v>
-      </c>
-      <c r="F179">
-        <v>35.40688883552489</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B180">
-        <v>2060</v>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E180">
-        <v>18820.74</v>
-      </c>
-      <c r="F180">
-        <v>2.92098525406861</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B181">
-        <v>2060</v>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E181">
-        <v>54304.7</v>
-      </c>
-      <c r="F181">
-        <v>8.428107923844634</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B182">
-        <v>2065</v>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E182">
-        <v>8590.48</v>
-      </c>
-      <c r="F182">
-        <v>1.328808137522934</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B183">
-        <v>2065</v>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D183" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E183">
-        <v>663.046735</v>
-      </c>
-      <c r="F183">
-        <v>0.1025625921981091</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B184">
-        <v>2065</v>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D184" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E184">
-        <v>320580</v>
-      </c>
-      <c r="F184">
-        <v>49.58853436910418</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B185">
-        <v>2065</v>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E185">
-        <v>247826.8</v>
-      </c>
-      <c r="F185">
-        <v>38.33479253036717</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B186">
-        <v>2065</v>
-      </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D186" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E186">
-        <v>16995.66</v>
-      </c>
-      <c r="F186">
-        <v>2.628953365885611</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B187">
-        <v>2065</v>
-      </c>
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D187" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E187">
-        <v>51824.1</v>
-      </c>
-      <c r="F187">
-        <v>8.016349004921992</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B188">
-        <v>2070</v>
-      </c>
-      <c r="C188" t="inlineStr">
-        <is>
-          <t>2W</t>
-        </is>
-      </c>
-      <c r="D188" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E188">
-        <v>6549.87</v>
-      </c>
-      <c r="F188">
-        <v>1.040163826624696</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B189">
-        <v>2070</v>
-      </c>
-      <c r="C189" t="inlineStr">
-        <is>
-          <t>3W</t>
-        </is>
-      </c>
-      <c r="D189" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E189">
-        <v>413.0190672</v>
-      </c>
-      <c r="F189">
-        <v>0.06559023208211989</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B190">
-        <v>2070</v>
-      </c>
-      <c r="C190" t="inlineStr">
-        <is>
-          <t>4W</t>
-        </is>
-      </c>
-      <c r="D190" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E190">
-        <v>311704</v>
-      </c>
-      <c r="F190">
-        <v>49.50071152774396</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B191">
-        <v>2070</v>
-      </c>
-      <c r="C191" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="D191" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E191">
-        <v>245214.72</v>
-      </c>
-      <c r="F191">
-        <v>38.94176243191139</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B192">
-        <v>2070</v>
-      </c>
-      <c r="C192" t="inlineStr">
-        <is>
-          <t>NMT</t>
-        </is>
-      </c>
-      <c r="D192" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E192">
-        <v>15646.69</v>
-      </c>
-      <c r="F192">
-        <v>2.484800605876204</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>Reference</t>
-        </is>
-      </c>
-      <c r="B193">
-        <v>2070</v>
-      </c>
-      <c r="C193" t="inlineStr">
-        <is>
-          <t>Rail</t>
-        </is>
-      </c>
-      <c r="D193" t="inlineStr">
-        <is>
-          <t>Passenger</t>
-        </is>
-      </c>
-      <c r="E193">
-        <v>50167.7</v>
-      </c>
-      <c r="F193">
-        <v>7.966971375761622</v>
+        <v>7.966976440162991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>